<commit_message>
Recognition time in native without jni
</commit_message>
<xml_diff>
--- a/Facemask results.xlsx
+++ b/Facemask results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\facemask\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9105"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.0\ _₽_-;\-* #,##0.0\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
@@ -272,9 +272,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -282,6 +279,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -301,7 +301,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -344,6 +344,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -444,6 +445,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -485,7 +487,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-78DB-4ED0-8059-247283569632}"/>
             </c:ext>
@@ -515,6 +517,65 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Images!$E$3</c:f>
@@ -527,7 +588,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000D-78DB-4ED0-8059-247283569632}"/>
             </c:ext>
@@ -597,6 +658,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -627,7 +689,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-78DB-4ED0-8059-247283569632}"/>
             </c:ext>
@@ -697,6 +759,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -727,7 +790,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000B-78DB-4ED0-8059-247283569632}"/>
             </c:ext>
@@ -797,6 +860,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -827,7 +891,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-78DB-4ED0-8059-247283569632}"/>
             </c:ext>
@@ -836,7 +900,7 @@
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -844,11 +908,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="261056808"/>
-        <c:axId val="261057136"/>
+        <c:axId val="171184376"/>
+        <c:axId val="173000856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="261056808"/>
+        <c:axId val="171184376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,7 +922,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261057136"/>
+        <c:crossAx val="173000856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -866,7 +930,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="261057136"/>
+        <c:axId val="173000856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -916,6 +980,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -976,7 +1041,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="261056808"/>
+        <c:crossAx val="171184376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -990,6 +1055,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1062,7 +1128,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1102,6 +1168,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1202,6 +1269,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1243,7 +1311,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9A1D-472D-A066-33B739F1E965}"/>
             </c:ext>
@@ -1273,6 +1341,65 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Images!$F$3</c:f>
@@ -1285,7 +1412,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-9A1D-472D-A066-33B739F1E965}"/>
             </c:ext>
@@ -1355,6 +1482,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1385,7 +1513,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9A1D-472D-A066-33B739F1E965}"/>
             </c:ext>
@@ -1455,6 +1583,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1485,7 +1614,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-9A1D-472D-A066-33B739F1E965}"/>
             </c:ext>
@@ -1555,6 +1684,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1585,15 +1715,16 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-9A1D-472D-A066-33B739F1E965}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1601,54 +1732,21 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="261056808"/>
-        <c:axId val="261057136"/>
+        <c:axId val="173025480"/>
+        <c:axId val="171393600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="261056808"/>
+        <c:axId val="173025480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="261057136"/>
+        <c:crossAx val="171393600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1656,7 +1754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="261057136"/>
+        <c:axId val="171393600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1706,6 +1804,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1766,7 +1865,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="261056808"/>
+        <c:crossAx val="173025480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1780,6 +1879,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1847,7 +1947,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1883,7 +1983,7 @@
               <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Recognition time dependency on size of images</a:t>
+              <a:t>Recognition time dependency on size of image</a:t>
             </a:r>
             <a:endParaRPr lang="ru-RU">
               <a:effectLst/>
@@ -1891,6 +1991,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1966,9 +2067,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Video!$B$3:$B$12</c:f>
+              <c:f>Video!$B$3:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>27x48</c:v>
                 </c:pt>
@@ -1998,6 +2099,36 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>270x480</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>297x528</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>324x576</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>351x624</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>378x672</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>405x720</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>432x768</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>459x816</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>486x864</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>513x912</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>540x960</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2072,7 +2203,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1EB0-4243-B115-644EA5114479}"/>
             </c:ext>
@@ -2116,6 +2247,74 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Video!$B$3:$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>27x48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54x96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81x144</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>108x192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>135x240</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>162x288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>189x336</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>216x384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>243x432</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>270x480</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>297x528</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>324x576</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>351x624</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>378x672</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>405x720</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>432x768</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>459x816</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>486x864</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>513x912</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>540x960</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Video!$E$3:$E$22</c:f>
@@ -2186,7 +2385,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-1EB0-4243-B115-644EA5114479}"/>
             </c:ext>
@@ -2232,9 +2431,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Video!$B$3:$B$12</c:f>
+              <c:f>Video!$B$3:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>27x48</c:v>
                 </c:pt>
@@ -2264,6 +2463,36 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>270x480</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>297x528</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>324x576</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>351x624</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>378x672</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>405x720</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>432x768</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>459x816</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>486x864</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>513x912</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>540x960</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2338,7 +2567,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1EB0-4243-B115-644EA5114479}"/>
             </c:ext>
@@ -2384,9 +2613,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Video!$B$3:$B$12</c:f>
+              <c:f>Video!$B$3:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>27x48</c:v>
                 </c:pt>
@@ -2416,6 +2645,36 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>270x480</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>297x528</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>324x576</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>351x624</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>378x672</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>405x720</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>432x768</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>459x816</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>486x864</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>513x912</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>540x960</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2490,7 +2749,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-1EB0-4243-B115-644EA5114479}"/>
             </c:ext>
@@ -2536,9 +2795,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Video!$B$3:$B$12</c:f>
+              <c:f>Video!$B$3:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>27x48</c:v>
                 </c:pt>
@@ -2568,6 +2827,36 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>270x480</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>297x528</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>324x576</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>351x624</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>378x672</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>405x720</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>432x768</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>459x816</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>486x864</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>513x912</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>540x960</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2642,14 +2931,13 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-1EB0-4243-B115-644EA5114479}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2659,11 +2947,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="518900792"/>
-        <c:axId val="518901776"/>
+        <c:axId val="173115216"/>
+        <c:axId val="173119696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="518900792"/>
+        <c:axId val="173115216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2714,6 +3002,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2780,7 +3069,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="518901776"/>
+        <c:crossAx val="173119696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2788,10 +3077,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="518901776"/>
+        <c:axId val="173119696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="500"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2854,6 +3142,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2914,7 +3203,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="518900792"/>
+        <c:crossAx val="173115216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3003,7 +3292,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3039,7 +3328,7 @@
               <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Recognition efficiency in dependency on size of images</a:t>
+              <a:t>Recognition efficiency in dependency on size of image</a:t>
             </a:r>
             <a:endParaRPr lang="ru-RU">
               <a:effectLst/>
@@ -3047,6 +3336,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3258,7 +3548,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B115-482F-8C96-3892F31D1419}"/>
             </c:ext>
@@ -3372,7 +3662,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-B115-482F-8C96-3892F31D1419}"/>
             </c:ext>
@@ -3554,7 +3844,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B115-482F-8C96-3892F31D1419}"/>
             </c:ext>
@@ -3736,7 +4026,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-B115-482F-8C96-3892F31D1419}"/>
             </c:ext>
@@ -3918,7 +4208,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-B115-482F-8C96-3892F31D1419}"/>
             </c:ext>
@@ -3934,11 +4224,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="518900792"/>
-        <c:axId val="518901776"/>
+        <c:axId val="173150160"/>
+        <c:axId val="173217192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="518900792"/>
+        <c:axId val="173150160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3989,6 +4279,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4055,7 +4346,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="518901776"/>
+        <c:crossAx val="173217192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4063,7 +4354,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="518901776"/>
+        <c:axId val="173217192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -4129,6 +4420,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4189,7 +4481,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="518900792"/>
+        <c:crossAx val="173150160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4278,7 +4570,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4322,6 +4614,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4397,38 +4690,38 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Video!$B$3:$B$12</c:f>
+              <c:f>Camera!$B$3:$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>27x48</c:v>
+                  <c:v>41x73</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54x96</c:v>
+                  <c:v>82x147</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81x144</c:v>
+                  <c:v>124x220</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108x192</c:v>
+                  <c:v>165x294</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>135x240</c:v>
+                  <c:v>207x368</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>162x288</c:v>
+                  <c:v>248x441</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>189x336</c:v>
+                  <c:v>289x515</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>216x384</c:v>
+                  <c:v>331x588</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>243x432</c:v>
+                  <c:v>372x662</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>270x480</c:v>
+                  <c:v>414x736</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4473,7 +4766,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2820-49B8-9C8E-9A1B0468035B}"/>
             </c:ext>
@@ -4519,38 +4812,38 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Video!$B$3:$B$12</c:f>
+              <c:f>Camera!$B$3:$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>27x48</c:v>
+                  <c:v>41x73</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54x96</c:v>
+                  <c:v>82x147</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81x144</c:v>
+                  <c:v>124x220</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108x192</c:v>
+                  <c:v>165x294</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>135x240</c:v>
+                  <c:v>207x368</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>162x288</c:v>
+                  <c:v>248x441</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>189x336</c:v>
+                  <c:v>289x515</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>216x384</c:v>
+                  <c:v>331x588</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>243x432</c:v>
+                  <c:v>372x662</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>270x480</c:v>
+                  <c:v>414x736</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4595,7 +4888,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2820-49B8-9C8E-9A1B0468035B}"/>
             </c:ext>
@@ -4613,6 +4906,7 @@
                   <c:v>GMS Vision</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4639,6 +4933,45 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Camera!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>41x73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82x147</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>124x220</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>165x294</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>207x368</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>248x441</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>289x515</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>331x588</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>372x662</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>414x736</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Camera!$G$3:$G$12</c:f>
@@ -4676,10 +5009,11 @@
                   <c:v>92.5</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-2820-49B8-9C8E-9A1B0468035B}"/>
             </c:ext>
@@ -4697,6 +5031,7 @@
                   <c:v>HAAR</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4725,40 +5060,41 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Video!$B$3:$B$12</c:f>
+              <c:f>Camera!$B$3:$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>27x48</c:v>
+                  <c:v>41x73</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54x96</c:v>
+                  <c:v>82x147</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81x144</c:v>
+                  <c:v>124x220</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108x192</c:v>
+                  <c:v>165x294</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>135x240</c:v>
+                  <c:v>207x368</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>162x288</c:v>
+                  <c:v>248x441</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>189x336</c:v>
+                  <c:v>289x515</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>216x384</c:v>
+                  <c:v>331x588</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>243x432</c:v>
+                  <c:v>372x662</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>270x480</c:v>
+                  <c:v>414x736</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:cat>
           <c:val>
@@ -4798,10 +5134,11 @@
                   <c:v>24.2</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-2820-49B8-9C8E-9A1B0468035B}"/>
             </c:ext>
@@ -4819,6 +5156,7 @@
                   <c:v>LBP</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4847,47 +5185,48 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Video!$B$3:$B$12</c:f>
+              <c:f>Camera!$B$3:$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>27x48</c:v>
+                  <c:v>41x73</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54x96</c:v>
+                  <c:v>82x147</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81x144</c:v>
+                  <c:v>124x220</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108x192</c:v>
+                  <c:v>165x294</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>135x240</c:v>
+                  <c:v>207x368</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>162x288</c:v>
+                  <c:v>248x441</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>189x336</c:v>
+                  <c:v>289x515</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>216x384</c:v>
+                  <c:v>331x588</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>243x432</c:v>
+                  <c:v>372x662</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>270x480</c:v>
+                  <c:v>414x736</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Camera!$K$3:$K$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -4920,10 +5259,11 @@
                   <c:v>7.2</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-2820-49B8-9C8E-9A1B0468035B}"/>
             </c:ext>
@@ -4939,11 +5279,12 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="518900792"/>
-        <c:axId val="518901776"/>
+        <c:axId val="173157776"/>
+        <c:axId val="169856504"/>
+        <c:extLst/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="518900792"/>
+        <c:axId val="173157776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4994,6 +5335,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5060,7 +5402,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="518901776"/>
+        <c:crossAx val="169856504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5068,7 +5410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="518901776"/>
+        <c:axId val="169856504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5133,6 +5475,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5193,7 +5536,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="518900792"/>
+        <c:crossAx val="173157776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8016,7 +8359,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E65900C4-3137-4914-AE3E-E1286A759E98}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E65900C4-3137-4914-AE3E-E1286A759E98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8052,7 +8395,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9414E354-1D0D-4DDD-BC92-CE89F215D114}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9414E354-1D0D-4DDD-BC92-CE89F215D114}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8076,21 +8419,21 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4467C4CB-071C-4E75-A7F1-DB9A317BFB13}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4467C4CB-071C-4E75-A7F1-DB9A317BFB13}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8112,21 +8455,21 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E839BA4E-74A7-475D-B3D7-350B8A74FFF6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E839BA4E-74A7-475D-B3D7-350B8A74FFF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8150,21 +8493,21 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>115</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31316556-0FBA-4D26-BA9C-A826EA09BDC8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31316556-0FBA-4D26-BA9C-A826EA09BDC8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8487,10 +8830,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8505,84 +8848,84 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="6"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2"/>
+      <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>29</v>
       </c>
       <c r="C3">
         <v>49.5</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>99</v>
       </c>
       <c r="E3">
@@ -8597,16 +8940,16 @@
       <c r="H3">
         <v>93.8</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>8.3000000000000007</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>100</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>2.5</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>100</v>
       </c>
     </row>
@@ -8629,772 +8972,772 @@
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2"/>
+      <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>1.2</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>10.199999999999999</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>0</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>9.3000000000000007</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>0</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>0.4</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>0</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>0.3</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>6.1</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>0</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>45.2</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>68</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>32</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>62</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>2.7</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>54.3</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>0.6</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>1.7</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>14.7</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>64.599999999999994</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>96.8</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>44.4</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>89.4</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>5.9</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>98.7</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>2.1</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>50.2</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>34.299999999999997</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>78</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>98.5</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>50.8</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>92.5</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>12.3</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>100</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>4.5</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <v>79.400000000000006</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>57.4</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>80.5</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>100</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>54.2</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>94</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>19.600000000000001</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>100</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>6</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <v>96.3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>76.099999999999994</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>33.299999999999997</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>80.900000000000006</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>99.2</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>57.4</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>93.5</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>22.5</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>100</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>7.6</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>103.2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>92.7</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>81</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>100</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>60.3</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>95.7</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>23.4</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>100</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>8.5</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>116.6</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>100</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>83.2</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>98.5</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>63.5</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>92.1</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>24.7</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>100</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>9.4</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>122</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>100</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>85.2</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>100</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>65.5</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>91.4</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="5">
         <v>26.3</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>100</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <v>10</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>150</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>100</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>87.4</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>100</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>72</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>97.2</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <v>25.8</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <v>100</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <v>10.6</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>179.3</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>100</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>88.1</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>100</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>72.3</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>94.4</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>28.6</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>100</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <v>11.1</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>191</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>100</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>93.4</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>100</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <v>77.400000000000006</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <v>93.4</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="5">
         <v>23.2</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>100</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>11.6</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>214.9</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>100</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>97.3</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>99.2</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>77.7</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <v>91.5</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="5">
         <v>22.5</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <v>100</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <v>11.9</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>225.1</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>100</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>103.3</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>100</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <v>85.8</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <v>97.6</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="5">
         <v>20.3</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="5">
         <v>100</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="5">
         <v>12.1</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>237</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>100</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>110.2</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>99.6</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>89.3</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>92.4</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <v>20.6</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>100</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>12.4</v>
       </c>
-      <c r="L17" s="6">
+      <c r="L17" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>261.2</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>100</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>116.2</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>99.1</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>96.7</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <v>92</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <v>21.8</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <v>100</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>13</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>299.89999999999998</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>100</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>120.7</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>100</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>104.8</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <v>94.5</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <v>22.4</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="5">
         <v>100</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="5">
         <v>14.4</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>316.39999999999998</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>100</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>131.9</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <v>100</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <v>109.2</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="5">
         <v>94.3</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="5">
         <v>23.2</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="5">
         <v>100</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K20" s="5">
         <v>15.2</v>
       </c>
-      <c r="L20" s="6">
+      <c r="L20" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>343.4</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>100</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>139.4</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <v>100</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <v>116.5</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <v>93.1</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="5">
         <v>24.7</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="5">
         <v>100</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="5">
         <v>15.3</v>
       </c>
-      <c r="L21" s="6">
+      <c r="L21" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>391.6</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>100</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>143.6</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <v>100</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="5">
         <v>123.1</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <v>97</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="5">
         <v>29.2</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="5">
         <v>100</v>
       </c>
-      <c r="K22" s="6">
+      <c r="K22" s="5">
         <v>15</v>
       </c>
-      <c r="L22" s="6">
+      <c r="L22" s="5">
         <v>100</v>
       </c>
     </row>
@@ -9415,329 +9758,329 @@
   <dimension ref="B1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2"/>
+      <c r="J1" s="6"/>
       <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>2.7</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
         <v>27.1</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5">
         <v>15.3</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5">
         <v>2.7</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6">
+      <c r="J3" s="5"/>
+      <c r="K3" s="5">
         <v>1</v>
       </c>
-      <c r="L3" s="6"/>
+      <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>32.5</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5">
         <v>38.700000000000003</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5">
         <v>19.899999999999999</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6">
+      <c r="H4" s="5"/>
+      <c r="I4" s="5">
         <v>7.5</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6">
+      <c r="J4" s="5"/>
+      <c r="K4" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>41.3</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5">
         <v>51.5</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5">
         <v>26.3</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6">
+      <c r="H5" s="5"/>
+      <c r="I5" s="5">
         <v>10.6</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6">
+      <c r="J5" s="5"/>
+      <c r="K5" s="5">
         <v>3.2</v>
       </c>
-      <c r="L5" s="6"/>
+      <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>52.3</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5">
         <v>65.3</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5">
         <v>31.8</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6">
+      <c r="H6" s="5"/>
+      <c r="I6" s="5">
         <v>10.6</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5">
         <v>4.3</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>103.5</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5">
         <v>73.900000000000006</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5">
         <v>41.2</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5">
         <v>11.1</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6">
+      <c r="J7" s="5"/>
+      <c r="K7" s="5">
         <v>5.2</v>
       </c>
-      <c r="L7" s="6"/>
+      <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>108.7</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5">
         <v>83.5</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5">
         <v>55.2</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5">
         <v>13.1</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6">
+      <c r="J8" s="5"/>
+      <c r="K8" s="5">
         <v>5.6</v>
       </c>
-      <c r="L8" s="6"/>
+      <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>123.2</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5">
         <v>91.3</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5">
         <v>64.3</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6">
+      <c r="H9" s="5"/>
+      <c r="I9" s="5">
         <v>13.7</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6">
+      <c r="J9" s="5"/>
+      <c r="K9" s="5">
         <v>6</v>
       </c>
-      <c r="L9" s="6"/>
+      <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>144</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5">
         <v>94.2</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5">
         <v>72.7</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6">
+      <c r="H10" s="5"/>
+      <c r="I10" s="5">
         <v>16.100000000000001</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6">
+      <c r="J10" s="5"/>
+      <c r="K10" s="5">
         <v>6.2</v>
       </c>
-      <c r="L10" s="6"/>
+      <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>167</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5">
         <v>109.1</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6">
+      <c r="F11" s="5"/>
+      <c r="G11" s="5">
         <v>81.8</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6">
+      <c r="H11" s="5"/>
+      <c r="I11" s="5">
         <v>19.8</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6">
+      <c r="J11" s="5"/>
+      <c r="K11" s="5">
         <v>6.7</v>
       </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>252</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5">
         <v>130.5</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6">
+      <c r="F12" s="5"/>
+      <c r="G12" s="5">
         <v>92.5</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5">
         <v>24.2</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6">
+      <c r="J12" s="5"/>
+      <c r="K12" s="5">
         <v>7.2</v>
       </c>
-      <c r="L12" s="6"/>
+      <c r="L12" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -9758,65 +10101,65 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2"/>
+      <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>50</v>
       </c>
@@ -9833,7 +10176,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>49</v>
       </c>
@@ -9850,7 +10193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>48</v>
       </c>
@@ -9867,87 +10210,87 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>31</v>
       </c>

</xml_diff>